<commit_message>
lab5 DONE. Maybe remove .xlsx file
</commit_message>
<xml_diff>
--- a/LABORATORY/LAB_3/route_space.xlsx
+++ b/LABORATORY/LAB_3/route_space.xlsx
@@ -1559,7 +1559,7 @@
         <v>3</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1570,7 +1570,7 @@
         <v>3</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1581,7 +1581,7 @@
         <v>3</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1592,7 +1592,7 @@
         <v>3</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1603,7 +1603,7 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1614,7 +1614,7 @@
         <v>3</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1625,7 +1625,7 @@
         <v>3</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1636,7 +1636,7 @@
         <v>3</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1647,7 +1647,7 @@
         <v>3</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1658,7 +1658,7 @@
         <v>3</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1669,7 +1669,7 @@
         <v>4</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1680,7 +1680,7 @@
         <v>4</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1691,7 +1691,7 @@
         <v>4</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1702,7 +1702,7 @@
         <v>4</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1713,7 +1713,7 @@
         <v>4</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1724,7 +1724,7 @@
         <v>4</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1735,7 +1735,7 @@
         <v>4</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1746,7 +1746,7 @@
         <v>4</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1757,7 +1757,7 @@
         <v>4</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1768,7 +1768,7 @@
         <v>4</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1779,7 +1779,7 @@
         <v>5</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1790,7 +1790,7 @@
         <v>5</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1801,7 +1801,7 @@
         <v>5</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1812,7 +1812,7 @@
         <v>5</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1823,7 +1823,7 @@
         <v>5</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1834,7 +1834,7 @@
         <v>5</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1845,7 +1845,7 @@
         <v>5</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1856,7 +1856,7 @@
         <v>5</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1867,7 +1867,7 @@
         <v>5</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1878,7 +1878,7 @@
         <v>5</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1889,7 +1889,7 @@
         <v>6</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1900,7 +1900,7 @@
         <v>6</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1911,7 +1911,7 @@
         <v>6</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1922,7 +1922,7 @@
         <v>6</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1933,7 +1933,7 @@
         <v>6</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1944,7 +1944,7 @@
         <v>6</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1955,7 +1955,7 @@
         <v>6</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1966,7 +1966,7 @@
         <v>6</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1977,7 +1977,7 @@
         <v>6</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1988,7 +1988,7 @@
         <v>6</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -2010,7 +2010,7 @@
         <v>7</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -2021,7 +2021,7 @@
         <v>7</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -2032,7 +2032,7 @@
         <v>7</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2043,7 +2043,7 @@
         <v>7</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -2054,7 +2054,7 @@
         <v>7</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -2065,7 +2065,7 @@
         <v>7</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -2076,7 +2076,7 @@
         <v>7</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -2087,7 +2087,7 @@
         <v>7</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2098,7 +2098,7 @@
         <v>7</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -2109,7 +2109,7 @@
         <v>8</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -2120,7 +2120,7 @@
         <v>8</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -2131,7 +2131,7 @@
         <v>8</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -2142,7 +2142,7 @@
         <v>8</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -2153,7 +2153,7 @@
         <v>8</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -2164,7 +2164,7 @@
         <v>8</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -2175,7 +2175,7 @@
         <v>8</v>
       </c>
       <c r="C68">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -2186,7 +2186,7 @@
         <v>8</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -2197,7 +2197,7 @@
         <v>8</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -2208,7 +2208,7 @@
         <v>8</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -2219,7 +2219,7 @@
         <v>9</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -2230,7 +2230,7 @@
         <v>9</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2241,7 +2241,7 @@
         <v>9</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2252,7 +2252,7 @@
         <v>9</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2263,7 +2263,7 @@
         <v>9</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2274,7 +2274,7 @@
         <v>9</v>
       </c>
       <c r="C77">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2285,7 +2285,7 @@
         <v>9</v>
       </c>
       <c r="C78">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2296,7 +2296,7 @@
         <v>9</v>
       </c>
       <c r="C79">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2307,7 +2307,7 @@
         <v>9</v>
       </c>
       <c r="C80">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -2318,7 +2318,7 @@
         <v>9</v>
       </c>
       <c r="C81">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2329,7 +2329,7 @@
         <v>10</v>
       </c>
       <c r="C82">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2351,7 +2351,7 @@
         <v>10</v>
       </c>
       <c r="C84">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2362,7 +2362,7 @@
         <v>10</v>
       </c>
       <c r="C85">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -2373,7 +2373,7 @@
         <v>10</v>
       </c>
       <c r="C86">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2384,7 +2384,7 @@
         <v>10</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2395,7 +2395,7 @@
         <v>10</v>
       </c>
       <c r="C88">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2406,7 +2406,7 @@
         <v>10</v>
       </c>
       <c r="C89">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2417,7 +2417,7 @@
         <v>10</v>
       </c>
       <c r="C90">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2428,7 +2428,7 @@
         <v>10</v>
       </c>
       <c r="C91">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2439,7 +2439,7 @@
         <v>11</v>
       </c>
       <c r="C92">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2450,7 +2450,7 @@
         <v>11</v>
       </c>
       <c r="C93">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2461,7 +2461,7 @@
         <v>11</v>
       </c>
       <c r="C94">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2472,7 +2472,7 @@
         <v>11</v>
       </c>
       <c r="C95">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2483,7 +2483,7 @@
         <v>11</v>
       </c>
       <c r="C96">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2494,7 +2494,7 @@
         <v>11</v>
       </c>
       <c r="C97">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2505,7 +2505,7 @@
         <v>11</v>
       </c>
       <c r="C98">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2516,7 +2516,7 @@
         <v>11</v>
       </c>
       <c r="C99">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2527,7 +2527,7 @@
         <v>11</v>
       </c>
       <c r="C100">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2538,7 +2538,7 @@
         <v>11</v>
       </c>
       <c r="C101">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2549,7 +2549,7 @@
         <v>12</v>
       </c>
       <c r="C102">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2560,7 +2560,7 @@
         <v>12</v>
       </c>
       <c r="C103">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2571,7 +2571,7 @@
         <v>12</v>
       </c>
       <c r="C104">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2582,7 +2582,7 @@
         <v>12</v>
       </c>
       <c r="C105">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2593,7 +2593,7 @@
         <v>12</v>
       </c>
       <c r="C106">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2604,7 +2604,7 @@
         <v>12</v>
       </c>
       <c r="C107">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2615,7 +2615,7 @@
         <v>12</v>
       </c>
       <c r="C108">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2626,7 +2626,7 @@
         <v>12</v>
       </c>
       <c r="C109">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2637,7 +2637,7 @@
         <v>12</v>
       </c>
       <c r="C110">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2648,7 +2648,7 @@
         <v>12</v>
       </c>
       <c r="C111">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2659,7 +2659,7 @@
         <v>13</v>
       </c>
       <c r="C112">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2670,7 +2670,7 @@
         <v>13</v>
       </c>
       <c r="C113">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2681,7 +2681,7 @@
         <v>13</v>
       </c>
       <c r="C114">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2692,7 +2692,7 @@
         <v>13</v>
       </c>
       <c r="C115">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2703,7 +2703,7 @@
         <v>13</v>
       </c>
       <c r="C116">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2714,7 +2714,7 @@
         <v>13</v>
       </c>
       <c r="C117">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2725,7 +2725,7 @@
         <v>13</v>
       </c>
       <c r="C118">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2736,7 +2736,7 @@
         <v>13</v>
       </c>
       <c r="C119">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2747,7 +2747,7 @@
         <v>13</v>
       </c>
       <c r="C120">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2758,7 +2758,7 @@
         <v>13</v>
       </c>
       <c r="C121">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -3979,7 +3979,7 @@
         <v>25</v>
       </c>
       <c r="C232">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -3990,7 +3990,7 @@
         <v>25</v>
       </c>
       <c r="C233">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -4001,7 +4001,7 @@
         <v>25</v>
       </c>
       <c r="C234">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -4012,7 +4012,7 @@
         <v>25</v>
       </c>
       <c r="C235">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -4023,7 +4023,7 @@
         <v>25</v>
       </c>
       <c r="C236">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="237" spans="1:3">
@@ -4034,7 +4034,7 @@
         <v>25</v>
       </c>
       <c r="C237">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -4045,7 +4045,7 @@
         <v>25</v>
       </c>
       <c r="C238">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -4056,7 +4056,7 @@
         <v>25</v>
       </c>
       <c r="C239">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -4067,7 +4067,7 @@
         <v>25</v>
       </c>
       <c r="C240">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -4078,7 +4078,7 @@
         <v>25</v>
       </c>
       <c r="C241">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -4969,7 +4969,7 @@
         <v>34</v>
       </c>
       <c r="C322">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="323" spans="1:3">
@@ -4980,7 +4980,7 @@
         <v>34</v>
       </c>
       <c r="C323">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="324" spans="1:3">
@@ -4991,7 +4991,7 @@
         <v>34</v>
       </c>
       <c r="C324">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="325" spans="1:3">
@@ -5002,7 +5002,7 @@
         <v>34</v>
       </c>
       <c r="C325">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="326" spans="1:3">
@@ -5013,7 +5013,7 @@
         <v>34</v>
       </c>
       <c r="C326">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="327" spans="1:3">
@@ -5024,7 +5024,7 @@
         <v>34</v>
       </c>
       <c r="C327">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="328" spans="1:3">
@@ -5035,7 +5035,7 @@
         <v>34</v>
       </c>
       <c r="C328">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="329" spans="1:3">
@@ -5046,7 +5046,7 @@
         <v>34</v>
       </c>
       <c r="C329">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="330" spans="1:3">
@@ -5057,7 +5057,7 @@
         <v>34</v>
       </c>
       <c r="C330">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="331" spans="1:3">
@@ -5068,7 +5068,7 @@
         <v>34</v>
       </c>
       <c r="C331">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="332" spans="1:3">
@@ -6289,7 +6289,7 @@
         <v>46</v>
       </c>
       <c r="C442">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="443" spans="1:3">
@@ -6300,7 +6300,7 @@
         <v>46</v>
       </c>
       <c r="C443">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="444" spans="1:3">
@@ -6311,7 +6311,7 @@
         <v>46</v>
       </c>
       <c r="C444">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="445" spans="1:3">
@@ -6322,7 +6322,7 @@
         <v>46</v>
       </c>
       <c r="C445">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="446" spans="1:3">
@@ -6333,7 +6333,7 @@
         <v>46</v>
       </c>
       <c r="C446">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="447" spans="1:3">
@@ -6344,7 +6344,7 @@
         <v>46</v>
       </c>
       <c r="C447">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="448" spans="1:3">
@@ -6355,7 +6355,7 @@
         <v>46</v>
       </c>
       <c r="C448">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="449" spans="1:3">
@@ -6366,7 +6366,7 @@
         <v>46</v>
       </c>
       <c r="C449">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="450" spans="1:3">
@@ -6377,7 +6377,7 @@
         <v>46</v>
       </c>
       <c r="C450">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="451" spans="1:3">
@@ -6388,7 +6388,7 @@
         <v>46</v>
       </c>
       <c r="C451">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="452" spans="1:3">
@@ -6509,7 +6509,7 @@
         <v>48</v>
       </c>
       <c r="C462">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="463" spans="1:3">
@@ -6520,7 +6520,7 @@
         <v>48</v>
       </c>
       <c r="C463">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="464" spans="1:3">
@@ -6531,7 +6531,7 @@
         <v>48</v>
       </c>
       <c r="C464">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="465" spans="1:3">
@@ -6542,7 +6542,7 @@
         <v>48</v>
       </c>
       <c r="C465">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="466" spans="1:3">
@@ -6553,7 +6553,7 @@
         <v>48</v>
       </c>
       <c r="C466">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="467" spans="1:3">
@@ -6564,7 +6564,7 @@
         <v>48</v>
       </c>
       <c r="C467">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="468" spans="1:3">
@@ -6575,7 +6575,7 @@
         <v>48</v>
       </c>
       <c r="C468">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="469" spans="1:3">
@@ -6586,7 +6586,7 @@
         <v>48</v>
       </c>
       <c r="C469">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="470" spans="1:3">
@@ -6597,7 +6597,7 @@
         <v>48</v>
       </c>
       <c r="C470">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="471" spans="1:3">
@@ -6608,7 +6608,7 @@
         <v>48</v>
       </c>
       <c r="C471">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="472" spans="1:3">
@@ -7169,7 +7169,7 @@
         <v>54</v>
       </c>
       <c r="C522">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="523" spans="1:3">
@@ -7180,7 +7180,7 @@
         <v>54</v>
       </c>
       <c r="C523">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="524" spans="1:3">
@@ -7191,7 +7191,7 @@
         <v>54</v>
       </c>
       <c r="C524">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="525" spans="1:3">
@@ -7202,7 +7202,7 @@
         <v>54</v>
       </c>
       <c r="C525">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="526" spans="1:3">
@@ -7213,7 +7213,7 @@
         <v>54</v>
       </c>
       <c r="C526">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="527" spans="1:3">
@@ -7224,7 +7224,7 @@
         <v>54</v>
       </c>
       <c r="C527">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="528" spans="1:3">
@@ -7235,7 +7235,7 @@
         <v>54</v>
       </c>
       <c r="C528">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="529" spans="1:3">
@@ -7246,7 +7246,7 @@
         <v>54</v>
       </c>
       <c r="C529">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="530" spans="1:3">
@@ -7257,7 +7257,7 @@
         <v>54</v>
       </c>
       <c r="C530">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="531" spans="1:3">
@@ -7268,7 +7268,7 @@
         <v>54</v>
       </c>
       <c r="C531">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="532" spans="1:3">
@@ -7499,7 +7499,7 @@
         <v>57</v>
       </c>
       <c r="C552">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="553" spans="1:3">
@@ -7510,7 +7510,7 @@
         <v>57</v>
       </c>
       <c r="C553">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="554" spans="1:3">
@@ -7521,7 +7521,7 @@
         <v>57</v>
       </c>
       <c r="C554">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="555" spans="1:3">
@@ -7532,7 +7532,7 @@
         <v>57</v>
       </c>
       <c r="C555">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="556" spans="1:3">
@@ -7543,7 +7543,7 @@
         <v>57</v>
       </c>
       <c r="C556">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="557" spans="1:3">
@@ -7554,7 +7554,7 @@
         <v>57</v>
       </c>
       <c r="C557">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="558" spans="1:3">
@@ -7565,7 +7565,7 @@
         <v>57</v>
       </c>
       <c r="C558">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="559" spans="1:3">
@@ -7576,7 +7576,7 @@
         <v>57</v>
       </c>
       <c r="C559">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="560" spans="1:3">
@@ -7587,7 +7587,7 @@
         <v>57</v>
       </c>
       <c r="C560">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="561" spans="1:3">
@@ -7598,7 +7598,7 @@
         <v>57</v>
       </c>
       <c r="C561">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="562" spans="1:3">
@@ -8049,7 +8049,7 @@
         <v>62</v>
       </c>
       <c r="C602">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="603" spans="1:3">
@@ -8060,7 +8060,7 @@
         <v>62</v>
       </c>
       <c r="C603">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="604" spans="1:3">
@@ -8071,7 +8071,7 @@
         <v>62</v>
       </c>
       <c r="C604">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="605" spans="1:3">
@@ -8082,7 +8082,7 @@
         <v>62</v>
       </c>
       <c r="C605">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="606" spans="1:3">
@@ -8093,7 +8093,7 @@
         <v>62</v>
       </c>
       <c r="C606">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="607" spans="1:3">
@@ -8104,7 +8104,7 @@
         <v>62</v>
       </c>
       <c r="C607">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="608" spans="1:3">
@@ -8115,7 +8115,7 @@
         <v>62</v>
       </c>
       <c r="C608">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="609" spans="1:3">
@@ -8126,7 +8126,7 @@
         <v>62</v>
       </c>
       <c r="C609">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="610" spans="1:3">
@@ -8137,7 +8137,7 @@
         <v>62</v>
       </c>
       <c r="C610">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="611" spans="1:3">
@@ -8148,7 +8148,7 @@
         <v>62</v>
       </c>
       <c r="C611">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="612" spans="1:3">
@@ -16409,7 +16409,7 @@
         <v>138</v>
       </c>
       <c r="C1362">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1363" spans="1:3">
@@ -16420,7 +16420,7 @@
         <v>138</v>
       </c>
       <c r="C1363">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1364" spans="1:3">
@@ -16431,7 +16431,7 @@
         <v>138</v>
       </c>
       <c r="C1364">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1365" spans="1:3">
@@ -16442,7 +16442,7 @@
         <v>138</v>
       </c>
       <c r="C1365">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1366" spans="1:3">
@@ -16453,7 +16453,7 @@
         <v>138</v>
       </c>
       <c r="C1366">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1367" spans="1:3">
@@ -16464,7 +16464,7 @@
         <v>138</v>
       </c>
       <c r="C1367">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1368" spans="1:3">
@@ -16475,7 +16475,7 @@
         <v>138</v>
       </c>
       <c r="C1368">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1369" spans="1:3">
@@ -16486,7 +16486,7 @@
         <v>138</v>
       </c>
       <c r="C1369">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1370" spans="1:3">
@@ -16497,7 +16497,7 @@
         <v>138</v>
       </c>
       <c r="C1370">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1371" spans="1:3">
@@ -16508,7 +16508,7 @@
         <v>138</v>
       </c>
       <c r="C1371">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1372" spans="1:3">
@@ -16959,7 +16959,7 @@
         <v>143</v>
       </c>
       <c r="C1412">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1413" spans="1:3">
@@ -16970,7 +16970,7 @@
         <v>143</v>
       </c>
       <c r="C1413">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1414" spans="1:3">
@@ -16981,7 +16981,7 @@
         <v>143</v>
       </c>
       <c r="C1414">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1415" spans="1:3">
@@ -16992,7 +16992,7 @@
         <v>143</v>
       </c>
       <c r="C1415">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1416" spans="1:3">
@@ -17003,7 +17003,7 @@
         <v>143</v>
       </c>
       <c r="C1416">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1417" spans="1:3">
@@ -17014,7 +17014,7 @@
         <v>143</v>
       </c>
       <c r="C1417">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1418" spans="1:3">
@@ -17025,7 +17025,7 @@
         <v>143</v>
       </c>
       <c r="C1418">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1419" spans="1:3">
@@ -17036,7 +17036,7 @@
         <v>143</v>
       </c>
       <c r="C1419">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1420" spans="1:3">
@@ -17047,7 +17047,7 @@
         <v>143</v>
       </c>
       <c r="C1420">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1421" spans="1:3">
@@ -17058,7 +17058,7 @@
         <v>143</v>
       </c>
       <c r="C1421">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1422" spans="1:3">
@@ -17509,7 +17509,7 @@
         <v>148</v>
       </c>
       <c r="C1462">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1463" spans="1:3">
@@ -17520,7 +17520,7 @@
         <v>148</v>
       </c>
       <c r="C1463">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1464" spans="1:3">
@@ -17531,7 +17531,7 @@
         <v>148</v>
       </c>
       <c r="C1464">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1465" spans="1:3">
@@ -17542,7 +17542,7 @@
         <v>148</v>
       </c>
       <c r="C1465">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1466" spans="1:3">
@@ -17553,7 +17553,7 @@
         <v>148</v>
       </c>
       <c r="C1466">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1467" spans="1:3">
@@ -17564,7 +17564,7 @@
         <v>148</v>
       </c>
       <c r="C1467">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1468" spans="1:3">
@@ -17575,7 +17575,7 @@
         <v>148</v>
       </c>
       <c r="C1468">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1469" spans="1:3">
@@ -17586,7 +17586,7 @@
         <v>148</v>
       </c>
       <c r="C1469">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1470" spans="1:3">
@@ -17597,7 +17597,7 @@
         <v>148</v>
       </c>
       <c r="C1470">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1471" spans="1:3">
@@ -17608,7 +17608,7 @@
         <v>148</v>
       </c>
       <c r="C1471">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1472" spans="1:3">
@@ -19819,7 +19819,7 @@
         <v>169</v>
       </c>
       <c r="C1672">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1673" spans="1:3">
@@ -19830,7 +19830,7 @@
         <v>169</v>
       </c>
       <c r="C1673">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1674" spans="1:3">
@@ -19841,7 +19841,7 @@
         <v>169</v>
       </c>
       <c r="C1674">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1675" spans="1:3">
@@ -19852,7 +19852,7 @@
         <v>169</v>
       </c>
       <c r="C1675">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1676" spans="1:3">
@@ -19863,7 +19863,7 @@
         <v>169</v>
       </c>
       <c r="C1676">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1677" spans="1:3">
@@ -19874,7 +19874,7 @@
         <v>169</v>
       </c>
       <c r="C1677">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1678" spans="1:3">
@@ -19885,7 +19885,7 @@
         <v>169</v>
       </c>
       <c r="C1678">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1679" spans="1:3">
@@ -19896,7 +19896,7 @@
         <v>169</v>
       </c>
       <c r="C1679">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1680" spans="1:3">
@@ -19907,7 +19907,7 @@
         <v>169</v>
       </c>
       <c r="C1680">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1681" spans="1:3">
@@ -19918,7 +19918,7 @@
         <v>169</v>
       </c>
       <c r="C1681">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1682" spans="1:3">
@@ -20919,7 +20919,7 @@
         <v>179</v>
       </c>
       <c r="C1772">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1773" spans="1:3">
@@ -20930,7 +20930,7 @@
         <v>179</v>
       </c>
       <c r="C1773">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1774" spans="1:3">
@@ -20941,7 +20941,7 @@
         <v>179</v>
       </c>
       <c r="C1774">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1775" spans="1:3">
@@ -20952,7 +20952,7 @@
         <v>179</v>
       </c>
       <c r="C1775">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1776" spans="1:3">
@@ -20963,7 +20963,7 @@
         <v>179</v>
       </c>
       <c r="C1776">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1777" spans="1:3">
@@ -20974,7 +20974,7 @@
         <v>179</v>
       </c>
       <c r="C1777">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1778" spans="1:3">
@@ -20985,7 +20985,7 @@
         <v>179</v>
       </c>
       <c r="C1778">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1779" spans="1:3">
@@ -20996,7 +20996,7 @@
         <v>179</v>
       </c>
       <c r="C1779">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1780" spans="1:3">
@@ -21007,7 +21007,7 @@
         <v>179</v>
       </c>
       <c r="C1780">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1781" spans="1:3">
@@ -21018,7 +21018,7 @@
         <v>179</v>
       </c>
       <c r="C1781">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1782" spans="1:3">
@@ -23339,7 +23339,7 @@
         <v>201</v>
       </c>
       <c r="C1992">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1993" spans="1:3">
@@ -23350,7 +23350,7 @@
         <v>201</v>
       </c>
       <c r="C1993">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1994" spans="1:3">
@@ -23361,7 +23361,7 @@
         <v>201</v>
       </c>
       <c r="C1994">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1995" spans="1:3">
@@ -23372,7 +23372,7 @@
         <v>201</v>
       </c>
       <c r="C1995">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1996" spans="1:3">
@@ -23383,7 +23383,7 @@
         <v>201</v>
       </c>
       <c r="C1996">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1997" spans="1:3">
@@ -23394,7 +23394,7 @@
         <v>201</v>
       </c>
       <c r="C1997">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1998" spans="1:3">
@@ -23405,7 +23405,7 @@
         <v>201</v>
       </c>
       <c r="C1998">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1999" spans="1:3">
@@ -23416,7 +23416,7 @@
         <v>201</v>
       </c>
       <c r="C1999">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2000" spans="1:3">
@@ -23427,7 +23427,7 @@
         <v>201</v>
       </c>
       <c r="C2000">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2001" spans="1:3">
@@ -23438,7 +23438,7 @@
         <v>201</v>
       </c>
       <c r="C2001">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2002" spans="1:3">
@@ -28839,7 +28839,7 @@
         <v>251</v>
       </c>
       <c r="C2492">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2493" spans="1:3">
@@ -28850,7 +28850,7 @@
         <v>251</v>
       </c>
       <c r="C2493">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2494" spans="1:3">
@@ -28861,7 +28861,7 @@
         <v>251</v>
       </c>
       <c r="C2494">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2495" spans="1:3">
@@ -28872,7 +28872,7 @@
         <v>251</v>
       </c>
       <c r="C2495">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2496" spans="1:3">
@@ -28883,7 +28883,7 @@
         <v>251</v>
       </c>
       <c r="C2496">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2497" spans="1:3">
@@ -28894,7 +28894,7 @@
         <v>251</v>
       </c>
       <c r="C2497">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2498" spans="1:3">
@@ -28905,7 +28905,7 @@
         <v>251</v>
       </c>
       <c r="C2498">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2499" spans="1:3">
@@ -28916,7 +28916,7 @@
         <v>251</v>
       </c>
       <c r="C2499">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2500" spans="1:3">
@@ -28927,7 +28927,7 @@
         <v>251</v>
       </c>
       <c r="C2500">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2501" spans="1:3">
@@ -28938,7 +28938,7 @@
         <v>251</v>
       </c>
       <c r="C2501">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2502" spans="1:3">
@@ -29389,7 +29389,7 @@
         <v>256</v>
       </c>
       <c r="C2542">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2543" spans="1:3">
@@ -29400,7 +29400,7 @@
         <v>256</v>
       </c>
       <c r="C2543">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2544" spans="1:3">
@@ -29411,7 +29411,7 @@
         <v>256</v>
       </c>
       <c r="C2544">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2545" spans="1:3">
@@ -29422,7 +29422,7 @@
         <v>256</v>
       </c>
       <c r="C2545">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2546" spans="1:3">
@@ -29433,7 +29433,7 @@
         <v>256</v>
       </c>
       <c r="C2546">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2547" spans="1:3">
@@ -29444,7 +29444,7 @@
         <v>256</v>
       </c>
       <c r="C2547">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2548" spans="1:3">
@@ -29455,7 +29455,7 @@
         <v>256</v>
       </c>
       <c r="C2548">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2549" spans="1:3">
@@ -29466,7 +29466,7 @@
         <v>256</v>
       </c>
       <c r="C2549">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2550" spans="1:3">
@@ -29477,7 +29477,7 @@
         <v>256</v>
       </c>
       <c r="C2550">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2551" spans="1:3">
@@ -29488,7 +29488,7 @@
         <v>256</v>
       </c>
       <c r="C2551">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2552" spans="1:3">
@@ -32909,7 +32909,7 @@
         <v>288</v>
       </c>
       <c r="C2862">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2863" spans="1:3">
@@ -32920,7 +32920,7 @@
         <v>288</v>
       </c>
       <c r="C2863">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2864" spans="1:3">
@@ -32931,7 +32931,7 @@
         <v>288</v>
       </c>
       <c r="C2864">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2865" spans="1:3">
@@ -32942,7 +32942,7 @@
         <v>288</v>
       </c>
       <c r="C2865">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2866" spans="1:3">
@@ -32953,7 +32953,7 @@
         <v>288</v>
       </c>
       <c r="C2866">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2867" spans="1:3">
@@ -32964,7 +32964,7 @@
         <v>288</v>
       </c>
       <c r="C2867">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2868" spans="1:3">
@@ -32975,7 +32975,7 @@
         <v>288</v>
       </c>
       <c r="C2868">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2869" spans="1:3">
@@ -32986,7 +32986,7 @@
         <v>288</v>
       </c>
       <c r="C2869">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2870" spans="1:3">
@@ -32997,7 +32997,7 @@
         <v>288</v>
       </c>
       <c r="C2870">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2871" spans="1:3">
@@ -33008,7 +33008,7 @@
         <v>288</v>
       </c>
       <c r="C2871">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2872" spans="1:3">
@@ -35769,7 +35769,7 @@
         <v>314</v>
       </c>
       <c r="C3122">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3123" spans="1:3">
@@ -35780,7 +35780,7 @@
         <v>314</v>
       </c>
       <c r="C3123">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3124" spans="1:3">
@@ -35791,7 +35791,7 @@
         <v>314</v>
       </c>
       <c r="C3124">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3125" spans="1:3">
@@ -35802,7 +35802,7 @@
         <v>314</v>
       </c>
       <c r="C3125">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3126" spans="1:3">
@@ -35813,7 +35813,7 @@
         <v>314</v>
       </c>
       <c r="C3126">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3127" spans="1:3">
@@ -35824,7 +35824,7 @@
         <v>314</v>
       </c>
       <c r="C3127">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3128" spans="1:3">
@@ -35835,7 +35835,7 @@
         <v>314</v>
       </c>
       <c r="C3128">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3129" spans="1:3">
@@ -35846,7 +35846,7 @@
         <v>314</v>
       </c>
       <c r="C3129">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3130" spans="1:3">
@@ -35857,7 +35857,7 @@
         <v>314</v>
       </c>
       <c r="C3130">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3131" spans="1:3">
@@ -35868,7 +35868,7 @@
         <v>314</v>
       </c>
       <c r="C3131">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3132" spans="1:3">

</xml_diff>